<commit_message>
Separati robula e robula+
</commit_message>
<xml_diff>
--- a/progetti-per-test/Progetto-html/confronto-pratiche.xlsx
+++ b/progetti-per-test/Progetto-html/confronto-pratiche.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Metodo di Generazione</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Applicazione: Progetto-html - Confronto Robustezza Locatori</t>
+  </si>
+  <si>
+    <t>robula+</t>
   </si>
 </sst>
 </file>
@@ -973,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1101,17 +1104,17 @@
         <v>40</v>
       </c>
       <c r="D7" s="3">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1119,23 +1122,23 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3">
         <v>40</v>
       </c>
       <c r="D8" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
+        <f>(E8/C8)*100</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1143,55 +1146,46 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>40</v>
       </c>
       <c r="D9" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>(E9/C9)*100</f>
+        <v>7.5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="3">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3">
-        <v>34</v>
-      </c>
-      <c r="E11" s="3">
-        <v>4</v>
-      </c>
-      <c r="F11" s="3">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" ref="G11:G16" si="1">(E11/C11)*100</f>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <f>(E10/C10)*100</f>
         <v>10</v>
       </c>
     </row>
@@ -1200,23 +1194,23 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3">
         <v>40</v>
       </c>
       <c r="D12" s="3">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E12" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f t="shared" ref="G12:G15" si="1">(E12/C12)*100</f>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1224,23 +1218,23 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3">
         <v>40</v>
       </c>
       <c r="D13" s="3">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E13" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
         <v>2</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1248,23 +1242,23 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3">
         <v>40</v>
       </c>
       <c r="D14" s="3">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1272,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3">
         <v>40</v>
@@ -1296,117 +1290,165 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3">
         <v>40</v>
       </c>
       <c r="D16" s="3">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3">
         <v>2</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="1"/>
+        <f>(E16/C16)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <f>(E17/C17)*100</f>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3">
+        <v>40</v>
+      </c>
+      <c r="D18" s="3">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
+        <f>(E18/C18)*100</f>
+        <v>7.5</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1">
-        <f>SUM(E4:E9)</f>
-        <v>29</v>
-      </c>
-      <c r="C20" s="1">
-        <f>SUM(F4:F9)</f>
-        <v>6</v>
-      </c>
-      <c r="D20" s="1">
-        <f>SUM(B20,C20)</f>
-        <v>35</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>9</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <f>SUM(E4:E10)</f>
+        <v>33</v>
+      </c>
+      <c r="C22" s="1">
+        <f>SUM(F4:F10)</f>
+        <v>7</v>
+      </c>
+      <c r="D22" s="1">
+        <f>SUM(B22,C22)</f>
+        <v>40</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>9</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="1">
-        <f>SUM(E11:E16)</f>
-        <v>28</v>
-      </c>
-      <c r="C21" s="1">
-        <f>SUM(F11:F16)</f>
-        <v>12</v>
-      </c>
-      <c r="D21" s="1">
-        <f>SUM(B21,C21)</f>
-        <v>40</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="B23" s="1">
+        <f>SUM(E12:E18)</f>
+        <v>31</v>
+      </c>
+      <c r="C23" s="1">
+        <f>SUM(F12:F18)</f>
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <f>SUM(B23,C23)</f>
+        <v>45</v>
+      </c>
+      <c r="E23" s="1">
         <v>0</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F23" s="1">
         <v>0</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G23" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>